<commit_message>
updated the menu with create and report, can now create parts
</commit_message>
<xml_diff>
--- a/GitHub Link & Scrum/RRS Scrum.xlsx
+++ b/GitHub Link & Scrum/RRS Scrum.xlsx
@@ -5,15 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelvu/Desktop/CSE/CSE1325/HW06/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelvu/Desktop/CSE/CSE1325/HW06/Robot/GitHub Link &amp; Scrum/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="440" yWindow="460" windowWidth="15360" windowHeight="10480" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
-    <sheet name="Sprint 1 Backlog" sheetId="2" r:id="rId2"/>
+    <sheet name="Sprint 4 Backlog" sheetId="2" r:id="rId2"/>
+    <sheet name="Sprint 5 Backlog" sheetId="4" r:id="rId3"/>
+    <sheet name="Sprint 6 Backlog" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="160">
   <si>
     <t>Product Name:</t>
   </si>
@@ -489,6 +491,27 @@
   </si>
   <si>
     <t>Create UML and Use Case Diagram</t>
+  </si>
+  <si>
+    <t>Updated Makefile with FLTK</t>
+  </si>
+  <si>
+    <t>Created FLTK Window</t>
+  </si>
+  <si>
+    <t>Created FLTK menu</t>
+  </si>
+  <si>
+    <t>Updated FLTK menu</t>
+  </si>
+  <si>
+    <t>Updated FLTK Window</t>
+  </si>
+  <si>
+    <t>Made code more efficient</t>
+  </si>
+  <si>
+    <t>Can create a part</t>
   </si>
 </sst>
 </file>
@@ -775,16 +798,16 @@
                   <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32.0</c:v>
+                  <c:v>31.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>32.0</c:v>
+                  <c:v>30.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>32.0</c:v>
+                  <c:v>30.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>32.0</c:v>
+                  <c:v>30.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -800,11 +823,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1108905312"/>
-        <c:axId val="-1089192800"/>
+        <c:axId val="-2069492736"/>
+        <c:axId val="-2068170784"/>
       </c:lineChart>
       <c:valAx>
-        <c:axId val="-1089192800"/>
+        <c:axId val="-2068170784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -859,12 +882,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1108905312"/>
+        <c:crossAx val="-2069492736"/>
         <c:crossesAt val="0.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="-1108905312"/>
+        <c:axId val="-2069492736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -909,7 +932,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1089192800"/>
+        <c:crossAx val="-2068170784"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -990,7 +1013,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 1 Backlog'!$B$6:$B$13</c:f>
+              <c:f>'Sprint 4 Backlog'!$B$6:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1032,11 +1055,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1089151472"/>
-        <c:axId val="-1089154864"/>
+        <c:axId val="-2068552880"/>
+        <c:axId val="-2068430352"/>
       </c:lineChart>
       <c:valAx>
-        <c:axId val="-1089154864"/>
+        <c:axId val="-2068430352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1091,12 +1114,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1089151472"/>
+        <c:crossAx val="-2068552880"/>
         <c:crossesAt val="0.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="-1089151472"/>
+        <c:axId val="-2068552880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1141,7 +1164,485 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1089154864"/>
+        <c:crossAx val="-2068430352"/>
+        <c:crossesAt val="0.0"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="B3B3B3"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1300" b="0"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Sprint Burn Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 5 Backlog'!$B$6:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="2113891264"/>
+        <c:axId val="2113804672"/>
+      </c:lineChart>
+      <c:valAx>
+        <c:axId val="2113804672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B3B3B3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Days</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="B3B3B3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2113891264"/>
+        <c:crossesAt val="0.0"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="2113891264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Tasks</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="B3B3B3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2113804672"/>
+        <c:crossesAt val="0.0"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="B3B3B3"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1300" b="0"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Sprint Burn Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 6 Backlog'!$B$6:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="-2070585872"/>
+        <c:axId val="-2066243808"/>
+      </c:lineChart>
+      <c:valAx>
+        <c:axId val="-2066243808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B3B3B3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Days</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="B3B3B3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2070585872"/>
+        <c:crossesAt val="0.0"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="-2070585872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Tasks</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="B3B3B3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2066243808"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1221,6 +1722,72 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="4086362" y="229697"/>
+    <xdr:ext cx="3751234" cy="1855043"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="shape">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9F5F4342-3C83-42E6-955A-3EAC06D9A310}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="4086362" y="229697"/>
+    <xdr:ext cx="3751234" cy="1855043"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="shape">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9F5F4342-3C83-42E6-955A-3EAC06D9A310}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1536,8 +2103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1854,7 +2421,7 @@
         <v>12</v>
       </c>
       <c r="B24" s="1">
-        <f t="shared" ref="B22:B29" si="1">B23</f>
+        <f t="shared" ref="B24:B29" si="1">B23</f>
         <v>32</v>
       </c>
       <c r="C24" s="3" t="s">
@@ -1878,7 +2445,7 @@
         <v>32</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D25" s="7">
         <f t="shared" si="0"/>
@@ -1894,11 +2461,10 @@
         <v>15</v>
       </c>
       <c r="B26" s="1">
-        <f t="shared" si="1"/>
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D26" s="7">
         <f t="shared" si="0"/>
@@ -1914,11 +2480,10 @@
         <v>16</v>
       </c>
       <c r="B27" s="1">
-        <f t="shared" si="1"/>
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D27" s="7">
         <f t="shared" si="0"/>
@@ -1935,7 +2500,7 @@
       </c>
       <c r="B28" s="1">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>14</v>
@@ -1955,7 +2520,7 @@
       </c>
       <c r="B29" s="1">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>14</v>
@@ -2035,6 +2600,12 @@
       <c r="B34">
         <v>1</v>
       </c>
+      <c r="C34" t="s">
+        <v>151</v>
+      </c>
+      <c r="D34">
+        <v>5</v>
+      </c>
       <c r="E34" s="11">
         <v>1</v>
       </c>
@@ -2074,6 +2645,12 @@
     <row r="36" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="B36">
         <v>3</v>
+      </c>
+      <c r="C36" t="s">
+        <v>151</v>
+      </c>
+      <c r="D36">
+        <v>6</v>
       </c>
       <c r="E36" s="11">
         <v>1</v>
@@ -2769,8 +3346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -2789,7 +3366,7 @@
         <v>23</v>
       </c>
       <c r="B1" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -3034,4 +3611,572 @@
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="9.5" customWidth="1"/>
+    <col min="2" max="4" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" customWidth="1"/>
+    <col min="6" max="6" width="48" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" customWidth="1"/>
+    <col min="8" max="8" width="48" customWidth="1"/>
+    <col min="9" max="1024" width="10.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B2" s="31">
+        <v>42674.875</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B3" s="31">
+        <v>42676.979166666664</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B4" s="31">
+        <v>42677.333333333336</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="1"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6" s="1">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B8" s="1">
+        <v>2</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B9" s="1">
+        <f t="shared" ref="B9:B11" si="0">B8</f>
+        <v>2</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B10" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B11" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A15" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="E16" t="s">
+        <v>149</v>
+      </c>
+      <c r="F16" t="s">
+        <v>153</v>
+      </c>
+      <c r="G16" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="17" spans="5:7" x14ac:dyDescent="0.15">
+      <c r="E17" t="s">
+        <v>149</v>
+      </c>
+      <c r="F17" t="s">
+        <v>154</v>
+      </c>
+      <c r="G17" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="18" spans="5:7" x14ac:dyDescent="0.15">
+      <c r="E18" t="s">
+        <v>149</v>
+      </c>
+      <c r="F18" t="s">
+        <v>155</v>
+      </c>
+      <c r="G18" t="s">
+        <v>151</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0" right="0" top="0.39370000000000011" bottom="0.39370000000000011" header="0" footer="0"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="9.5" customWidth="1"/>
+    <col min="2" max="4" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" customWidth="1"/>
+    <col min="6" max="6" width="48" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" customWidth="1"/>
+    <col min="8" max="8" width="48" customWidth="1"/>
+    <col min="9" max="1024" width="10.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B2" s="31">
+        <v>42680.875</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B3" s="31">
+        <v>42683.979166666664</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B4" s="31">
+        <v>42684.333333333336</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="1"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6" s="1">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B7" s="1">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B8" s="1">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B10" s="1">
+        <f t="shared" ref="B9:B11" si="0">B9</f>
+        <v>2</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B11" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A15" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="E16" t="s">
+        <v>149</v>
+      </c>
+      <c r="F16" t="s">
+        <v>158</v>
+      </c>
+      <c r="G16" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="17" spans="5:7" x14ac:dyDescent="0.15">
+      <c r="E17" t="s">
+        <v>149</v>
+      </c>
+      <c r="F17" t="s">
+        <v>157</v>
+      </c>
+      <c r="G17" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="18" spans="5:7" x14ac:dyDescent="0.15">
+      <c r="E18" t="s">
+        <v>149</v>
+      </c>
+      <c r="F18" t="s">
+        <v>156</v>
+      </c>
+      <c r="G18" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="19" spans="5:7" x14ac:dyDescent="0.15">
+      <c r="E19" t="s">
+        <v>149</v>
+      </c>
+      <c r="F19" t="s">
+        <v>159</v>
+      </c>
+      <c r="G19" t="s">
+        <v>151</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0" right="0" top="0.39370000000000011" bottom="0.39370000000000011" header="0" footer="0"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added features to GUI
</commit_message>
<xml_diff>
--- a/GitHub Link & Scrum/RRS Scrum.xlsx
+++ b/GitHub Link & Scrum/RRS Scrum.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -2103,7 +2103,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I71"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
@@ -3896,7 +3896,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>

</xml_diff>